<commit_message>
additional columns added to example input file
</commit_message>
<xml_diff>
--- a/example_input_files/example_multisheet_chr-start-end_input.xlsx
+++ b/example_input_files/example_multisheet_chr-start-end_input.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
@@ -21,9 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t xml:space="preserve">Gene location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other data</t>
   </si>
   <si>
     <t xml:space="preserve">chr2:47930149-48320174</t>
@@ -32,10 +35,22 @@
     <t xml:space="preserve">chr16:2298327-2363113</t>
   </si>
   <si>
+    <t xml:space="preserve">other data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random</t>
+  </si>
+  <si>
     <t xml:space="preserve">chr20:25070421-25122324</t>
   </si>
   <si>
+    <t xml:space="preserve">xyz</t>
+  </si>
+  <si>
     <t xml:space="preserve">chr3:38459967-38499186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abc</t>
   </si>
 </sst>
 </file>
@@ -133,24 +148,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -343,31 +362,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:A15"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -386,27 +414,48 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A596"/>
+  <dimension ref="A1:C596"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A4:A15"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.04"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>3</v>
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>4</v>
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -457,7 +506,7 @@
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="3"/>
+      <c r="A51" s="4"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -576,7 +625,7 @@
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="3"/>
+      <c r="A168" s="4"/>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -763,12 +812,12 @@
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A353" s="4"/>
+      <c r="A353" s="5"/>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A356" s="4"/>
+      <c r="A356" s="5"/>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>